<commit_message>
adicionei o gráfico de gastos de caçapava
</commit_message>
<xml_diff>
--- a/Dados/Dados de gastos/Cacapava/gastos2019-2022.xlsx
+++ b/Dados/Dados de gastos/Cacapava/gastos2019-2022.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Fatec\API\Cacapava\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/120fd542a8b8b6a0/Área de Trabalho/API/Dados/Dados de gastos/Cacapava/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_58DF2BC0F5852B3CC18EFAC0CC022426EE566473" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FA25220-AFF2-4D34-94DB-B583A9E85472}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -26,16 +38,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>investimento em saúde</t>
+    <t>ano</t>
   </si>
   <si>
-    <t>ano</t>
+    <t>Aplicação de recursos na saúde por ano</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -121,7 +133,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -135,6 +147,1166 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15579530214709672"/>
+          <c:y val="0.17647798742138365"/>
+          <c:w val="0.8164690417070547"/>
+          <c:h val="0.63734462437478323"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Aplicação de recursos na saúde por ano</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-09E1-42F0-825F-5DD497B51269}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-09E1-42F0-825F-5DD497B51269}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-09E1-42F0-825F-5DD497B51269}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:numRef>
+              <c:f>Planilha1!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2022</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>56519952.170000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>108731494</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72271852.540000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72919950.269999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-09E1-42F0-825F-5DD497B51269}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1426187631"/>
+        <c:axId val="1426180911"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Planilha1!$B$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>ano</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Planilha1!$B$2:$B$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>2019</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2020</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2021</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2022</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Planilha1!$B$2:$B$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>2019</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2020</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2021</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2022</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-09E1-42F0-825F-5DD497B51269}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1426187631"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Ano</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1426180911"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1426180911"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Gasto</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-BR" baseline="0"/>
+                  <a:t> em milhões (R$)</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1426187631"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+        </c:dispUnits>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1088C8FF-F104-09D1-930F-91DD8D795FB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -399,24 +1571,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -454,5 +1626,6 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>